<commit_message>
if, nested if, and, or condition done
</commit_message>
<xml_diff>
--- a/Practice/day1.xlsx
+++ b/Practice/day1.xlsx
@@ -33,7 +33,7 @@
     <definedName name="Suresh" localSheetId="4">'sumif sumifs'!$D$2:$G$2</definedName>
     <definedName name="Suresh">'Name Manager'!$D$2:$G$2</definedName>
   </definedNames>
-  <calcPr calcId="152511"/>
+  <calcPr calcId="162913"/>
 </workbook>
 </file>
 
@@ -139,7 +139,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -701,7 +701,7 @@
   <dimension ref="A1:M15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M11" sqref="M11"/>
+      <selection sqref="A1:I11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1104,7 +1104,7 @@
       <c r="A2" s="13"/>
       <c r="B2" s="13">
         <f ca="1">TODAY()</f>
-        <v>45195</v>
+        <v>45196</v>
       </c>
       <c r="D2" s="13">
         <v>45194</v>

</xml_diff>